<commit_message>
Update a question text and commented out the image column in Item model
</commit_message>
<xml_diff>
--- a/itemBank.xlsx
+++ b/itemBank.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/richard.holliday/repos/python/Grade-12-Final/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C43FD81-F6A3-E042-B795-35A27B34BF61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF422155-1374-AB4F-9BEB-DE1CA29FF902}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5360" yWindow="500" windowWidth="27120" windowHeight="23720" xr2:uid="{AD11A411-9A43-5748-99D7-C3C574C8B868}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17500" xr2:uid="{AD11A411-9A43-5748-99D7-C3C574C8B868}"/>
   </bookViews>
   <sheets>
     <sheet name="itemBank" sheetId="1" r:id="rId1"/>
@@ -146,12 +146,6 @@
     <t>School</t>
   </si>
   <si>
-    <t>What is a group of crows called?</t>
-  </si>
-  <si>
-    <t>Murder</t>
-  </si>
-  <si>
     <t>La couleur d'une pomme est ?</t>
   </si>
   <si>
@@ -246,6 +240,12 @@
   </si>
   <si>
     <t>C'est quoi ce mot : souris ?\tRat\tCat\tMouse\tSnake</t>
+  </si>
+  <si>
+    <t>Is it "I have less photos than last year" or "I have fewer photos than last year"</t>
+  </si>
+  <si>
+    <t>fewer</t>
   </si>
 </sst>
 </file>
@@ -301,9 +301,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -341,7 +341,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -447,7 +447,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -589,7 +589,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -599,8 +599,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40DC7A7E-E0CC-674C-A00B-05982561C046}">
   <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="32" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -789,10 +789,10 @@
         <v>8</v>
       </c>
       <c r="C11" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D11" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E11">
         <v>0.5</v>
@@ -806,10 +806,10 @@
         <v>8</v>
       </c>
       <c r="C12" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D12" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E12">
         <v>0.5</v>
@@ -823,10 +823,10 @@
         <v>8</v>
       </c>
       <c r="C13" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D13" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E13">
         <v>0.5</v>
@@ -840,10 +840,10 @@
         <v>8</v>
       </c>
       <c r="C14" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D14" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E14">
         <v>0.5</v>
@@ -857,10 +857,10 @@
         <v>8</v>
       </c>
       <c r="C15" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D15" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E15">
         <v>0.5</v>
@@ -874,10 +874,10 @@
         <v>8</v>
       </c>
       <c r="C16" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D16" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E16">
         <v>0.5</v>
@@ -891,10 +891,10 @@
         <v>8</v>
       </c>
       <c r="C17" t="s">
+        <v>58</v>
+      </c>
+      <c r="D17" t="s">
         <v>60</v>
-      </c>
-      <c r="D17" t="s">
-        <v>62</v>
       </c>
       <c r="E17">
         <v>0.5</v>
@@ -908,10 +908,10 @@
         <v>8</v>
       </c>
       <c r="C18" t="s">
+        <v>59</v>
+      </c>
+      <c r="D18" t="s">
         <v>61</v>
-      </c>
-      <c r="D18" t="s">
-        <v>63</v>
       </c>
       <c r="E18">
         <v>0.5</v>
@@ -925,10 +925,10 @@
         <v>8</v>
       </c>
       <c r="C19" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D19" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E19">
         <v>0.5</v>
@@ -942,10 +942,10 @@
         <v>8</v>
       </c>
       <c r="C20" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D20" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E20">
         <v>0.5</v>
@@ -959,10 +959,10 @@
         <v>8</v>
       </c>
       <c r="C21" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D21" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E21">
         <v>0.5</v>
@@ -1044,10 +1044,10 @@
         <v>9</v>
       </c>
       <c r="C26" t="s">
-        <v>36</v>
+        <v>68</v>
       </c>
       <c r="D26" t="s">
-        <v>37</v>
+        <v>69</v>
       </c>
       <c r="E26">
         <v>0.5</v>
@@ -1061,10 +1061,10 @@
         <v>9</v>
       </c>
       <c r="C27" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D27" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E27">
         <v>0.5</v>
@@ -1078,10 +1078,10 @@
         <v>9</v>
       </c>
       <c r="C28" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D28" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E28">
         <v>0.5</v>
@@ -1095,10 +1095,10 @@
         <v>9</v>
       </c>
       <c r="C29" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D29" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E29">
         <v>0.5</v>
@@ -1112,10 +1112,10 @@
         <v>9</v>
       </c>
       <c r="C30" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D30" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E30">
         <v>0.5</v>
@@ -1129,10 +1129,10 @@
         <v>9</v>
       </c>
       <c r="C31" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D31" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E31">
         <v>0.5</v>

</xml_diff>